<commit_message>
Test loading of xls and xlsx with shared formulas.
To make sure I won't break this.  And I moved the xlsx version of the
test from the slow check to the normal test, which gets run for the normal
build target.

Change-Id: Id65f79796b11c0ab039842f1c1c158e9af310757
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/shared-formula.xlsx
+++ b/sc/qa/unit/data/xlsx/shared-formula.xlsx
@@ -1,29 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="28560" windowHeight="14385"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="14355" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,69 +350,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2">
-        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2*10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <f t="shared" ref="A3:A9" si="0">A2+1</f>
+      <c r="B3">
+        <f t="shared" ref="B3:B19" si="0">A3*10</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <f t="shared" si="0"/>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5">
-        <f t="shared" si="0"/>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6">
-        <f t="shared" si="0"/>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7">
-        <f t="shared" si="0"/>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8">
-        <f t="shared" si="0"/>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9">
-        <f t="shared" si="0"/>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -414,9 +541,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -426,8 +555,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>